<commit_message>
added drill and boxing glove to ideas
</commit_message>
<xml_diff>
--- a/Ideas.xlsx
+++ b/Ideas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\CS447-Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6593411a8a2fd1c/Desktop/WSU/CS 447/project2/CS447-Project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD5BC7-6C8E-47EF-ACBD-070ED6767E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{12CD5BC7-6C8E-47EF-ACBD-070ED6767E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{44DBF8BD-DB5C-47BF-AD33-CE9AB70642FB}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1275" windowWidth="23700" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Idea Name</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>No plans to implement</t>
+  </si>
+  <si>
+    <t>Drill</t>
+  </si>
+  <si>
+    <t>Utility/Movement</t>
+  </si>
+  <si>
+    <t>When activated, the tank using it moves in a user-specified direction, destroying terrain in its path for a set time. Gravity affects the tank as usual while the item is activated, to prevent tanks from using the drill to fly.</t>
+  </si>
+  <si>
+    <t>Ben: Feels like a given once we get destructable terrain working. Sufficiently unique experience to be meet complexity requirement.</t>
+  </si>
+  <si>
+    <t>Boxing Glove</t>
+  </si>
+  <si>
+    <t>A Melee weapon that has short range and low damage, but high knockback.</t>
   </si>
 </sst>
 </file>
@@ -563,23 +581,24 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="11" customWidth="1"/>
     <col min="4" max="4" width="15" style="17" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="18"/>
-    <col min="6" max="6" width="99.28515625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="15"/>
-    <col min="10" max="16384" width="9.140625" style="15"/>
+    <col min="5" max="5" width="9.1796875" style="18"/>
+    <col min="6" max="6" width="99.26953125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="15"/>
+    <col min="9" max="9" width="8.7265625" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -626,19 +645,52 @@
       </c>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="G3" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="G4" s="19" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G5" s="20" t="s">
         <v>15</v>
       </c>

</xml_diff>